<commit_message>
Changed threshold for UmeaBitBlasterSiblingBundling
</commit_message>
<xml_diff>
--- a/src/main/resources/Thresholds.xlsx
+++ b/src/main/resources/Thresholds.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/al/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/al/repos/github/population-linkage/src/main/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AAE85CCE-08AB-6646-A3F6-A48C078D598A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57142C47-5C60-2B4F-9DE1-9472E80E558A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34440" yWindow="11760" windowWidth="28040" windowHeight="17440" xr2:uid="{7B9943E8-D275-234A-B608-D54B29672835}"/>
+    <workbookView xWindow="780" yWindow="8320" windowWidth="35460" windowHeight="19200" activeTab="1" xr2:uid="{7B9943E8-D275-234A-B608-D54B29672835}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="139">
   <si>
     <t>UmeaBirthFatherPRFByThreshold.csv</t>
   </si>
@@ -433,14 +433,23 @@
     <t>Sum Unormalised threshold</t>
   </si>
   <si>
-    <t>From running PrintPwerTable.R</t>
+    <t>From running PrintPowerTable.R</t>
+  </si>
+  <si>
+    <t>thresh/fields</t>
+  </si>
+  <si>
+    <t>FRobustness2</t>
+  </si>
+  <si>
+    <t>or</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -456,8 +465,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <i/>
+      <sz val="11.3"/>
+      <color rgb="FF808080"/>
+      <name val="Menlo"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -467,6 +483,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -483,10 +505,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -801,10 +825,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07F3C972-797E-CE4F-B166-6A5F814F46C6}">
-  <dimension ref="A1:D166"/>
+  <dimension ref="A1:F166"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+    <sheetView zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A133" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D136" sqref="D136"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -815,7 +840,7 @@
     <col min="4" max="4" width="24.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>131</v>
       </c>
@@ -828,8 +853,11 @@
       <c r="D1" s="1" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F1" s="2" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -843,7 +871,7 @@
         <v>0.13636363636363599</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -857,7 +885,7 @@
         <v>5.2631578947368397E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -871,7 +899,7 @@
         <v>0.31578947368421101</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>0</v>
       </c>
@@ -885,7 +913,7 @@
         <v>0.31578947368421101</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>0</v>
       </c>
@@ -899,7 +927,7 @@
         <v>0.35135135135135098</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>0</v>
       </c>
@@ -913,7 +941,7 @@
         <v>0.29870129870129902</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>0</v>
       </c>
@@ -927,7 +955,7 @@
         <v>6.3829787234042507E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>0</v>
       </c>
@@ -941,7 +969,7 @@
         <v>0.28205128205128199</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>0</v>
       </c>
@@ -955,7 +983,7 @@
         <v>0.17647058823529399</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>0</v>
       </c>
@@ -969,7 +997,7 @@
         <v>0.58730158730158699</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>0</v>
       </c>
@@ -983,7 +1011,7 @@
         <v>0.11111111111111099</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>0</v>
       </c>
@@ -997,7 +1025,7 @@
         <v>8.6956521739130405E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>0</v>
       </c>
@@ -1011,7 +1039,7 @@
         <v>0.20481927710843401</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>0</v>
       </c>
@@ -1025,7 +1053,7 @@
         <v>1.38095238095238</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>0</v>
       </c>
@@ -2607,7 +2635,7 @@
         <v>1.27272727272727</v>
       </c>
     </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
         <v>128</v>
       </c>
@@ -2621,7 +2649,7 @@
         <v>1.1739130434782601</v>
       </c>
     </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
         <v>128</v>
       </c>
@@ -2635,7 +2663,7 @@
         <v>1.7027027027027</v>
       </c>
     </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
         <v>128</v>
       </c>
@@ -2649,7 +2677,7 @@
         <v>1.6315789473684199</v>
       </c>
     </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
         <v>128</v>
       </c>
@@ -2663,7 +2691,7 @@
         <v>2.3333333333333299</v>
       </c>
     </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
         <v>128</v>
       </c>
@@ -2677,7 +2705,7 @@
         <v>2.3333333333333299</v>
       </c>
     </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
         <v>128</v>
       </c>
@@ -2691,7 +2719,7 @@
         <v>1.8571428571428601</v>
       </c>
     </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
         <v>128</v>
       </c>
@@ -2705,21 +2733,25 @@
         <v>2.125</v>
       </c>
     </row>
-    <row r="136" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A136" t="s">
+    <row r="136" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A136" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="B136" t="s">
+      <c r="B136" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="C136">
+      <c r="C136" s="3">
         <v>9.7100000000000009</v>
       </c>
-      <c r="D136">
+      <c r="D136" s="3">
         <v>2.0303030303030298</v>
       </c>
-    </row>
-    <row r="137" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F136" s="3">
+        <f>D136/8</f>
+        <v>0.25378787878787873</v>
+      </c>
+    </row>
+    <row r="137" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
         <v>129</v>
       </c>
@@ -2733,7 +2765,7 @@
         <v>0.35135135135135098</v>
       </c>
     </row>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
         <v>129</v>
       </c>
@@ -2747,7 +2779,7 @@
         <v>15.6666666666667</v>
       </c>
     </row>
-    <row r="139" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
         <v>129</v>
       </c>
@@ -2761,7 +2793,7 @@
         <v>6.6923076923076898</v>
       </c>
     </row>
-    <row r="140" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
         <v>129</v>
       </c>
@@ -2775,7 +2807,7 @@
         <v>6.6923076923076898</v>
       </c>
     </row>
-    <row r="141" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
         <v>129</v>
       </c>
@@ -2789,7 +2821,7 @@
         <v>0.42857142857142899</v>
       </c>
     </row>
-    <row r="142" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
         <v>129</v>
       </c>
@@ -2803,7 +2835,7 @@
         <v>0.51515151515151503</v>
       </c>
     </row>
-    <row r="143" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
         <v>129</v>
       </c>
@@ -2817,7 +2849,7 @@
         <v>0.69491525423728795</v>
       </c>
     </row>
-    <row r="144" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
         <v>129</v>
       </c>
@@ -3146,17 +3178,25 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{129342A9-B6F4-304E-AA1B-3B24FFFFFAE3}">
-  <dimension ref="A4"/>
+  <dimension ref="A4:D5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>135</v>
+      </c>
+      <c r="D4" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="4" t="s">
+        <v>137</v>
       </c>
     </row>
   </sheetData>

</xml_diff>